<commit_message>
Fix typo in core 13 weight on 2019-03-14
</commit_message>
<xml_diff>
--- a/data/cpcrw-cores-picarro-mass-track.xlsx
+++ b/data/cpcrw-cores-picarro-mass-track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d3x290/Documents/Work/Current/Bailey SFA/2019/TES-drydown/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEB39F9-DBC7-3942-9D02-B46456E9B511}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3A392F-07E2-9A40-A9C6-5BA70C82039B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="460" windowWidth="24740" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -699,8 +699,8 @@
   <dimension ref="A1:Y1964"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A981" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G998" sqref="G998"/>
+      <pane ySplit="1" topLeftCell="A879" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G886" sqref="G886"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -35675,7 +35675,7 @@
         <v>15</v>
       </c>
       <c r="G885" s="1">
-        <v>109.76</v>
+        <v>190.76</v>
       </c>
       <c r="H885" s="2"/>
       <c r="I885" s="2"/>

</xml_diff>